<commit_message>
implimented save, export, view upload, collating of results
</commit_message>
<xml_diff>
--- a/sample_input_data/Sample_result.xlsx
+++ b/sample_input_data/Sample_result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Olaye Pav 2020\Projects2021\Result_and_Transcript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp7.4\htdocs\result_and_transcript_system\desktop_src\result_and_transcript_system\result_and_transcript_system\bin\Debug\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>CA</t>
   </si>
@@ -57,20 +57,83 @@
     <t>UNIVERSITY NAME</t>
   </si>
   <si>
-    <t>CPE300: Artificial Inteligence</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
     <t>GRADE</t>
+  </si>
+  <si>
+    <t>ENG1503585</t>
+  </si>
+  <si>
+    <t>ENG1503586</t>
+  </si>
+  <si>
+    <t>ENG1503587</t>
+  </si>
+  <si>
+    <t>ENG1503588</t>
+  </si>
+  <si>
+    <t>ENG1503589</t>
+  </si>
+  <si>
+    <t>ENG1503590</t>
+  </si>
+  <si>
+    <t>ENG1503591</t>
+  </si>
+  <si>
+    <t>ENG1503592</t>
+  </si>
+  <si>
+    <t>ENG1503593</t>
+  </si>
+  <si>
+    <t>ENG1503594</t>
+  </si>
+  <si>
+    <t>ENG1503595</t>
+  </si>
+  <si>
+    <t>ENG1503596</t>
+  </si>
+  <si>
+    <t>ENG1503597</t>
+  </si>
+  <si>
+    <t>ENG1503598</t>
+  </si>
+  <si>
+    <t>ENG1503599</t>
+  </si>
+  <si>
+    <t>ENG1503226</t>
+  </si>
+  <si>
+    <t>ENG1503227</t>
+  </si>
+  <si>
+    <t>ENG1503228</t>
+  </si>
+  <si>
+    <t>ENG1502299</t>
+  </si>
+  <si>
+    <t>CPE314: Electromagnetism</t>
+  </si>
+  <si>
+    <t>Optional Name SURNAME</t>
+  </si>
+  <si>
+    <t>Optional Name2 SURNAME (Miss)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +147,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -106,24 +177,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -142,7 +200,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -155,11 +215,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -170,10 +232,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,65 +550,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H85"/>
+  <dimension ref="B1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -548,1426 +620,2027 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>1102290</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7">
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="8">
         <v>4</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="8">
         <v>46</v>
       </c>
       <c r="G9" s="8">
         <f>E9+F9</f>
         <v>50</v>
       </c>
+      <c r="H9" s="9" t="str">
+        <f>IF(G9="","",IF(G9&lt;40,"F",IF(G9&lt;45,"E",IF(G9&lt;50,"D",IF(G9&lt;60,"C",IF(G9&lt;70,"B",IF(G9&lt;101,"A",IF(G9="","","ABS"))))))))</f>
+        <v>C</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+      <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="C10" s="5">
-        <v>1202894</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5">
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="10">
         <v>10</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="10">
         <v>66</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="10">
         <f t="shared" ref="G10:G73" si="0">E10+F10</f>
         <v>76</v>
       </c>
+      <c r="H10" s="9" t="str">
+        <f t="shared" ref="H10:H73" si="1">IF(G10="","",IF(G10&lt;40,"F",IF(G10&lt;45,"E",IF(G10&lt;50,"D",IF(G10&lt;60,"C",IF(G10&lt;70,"B",IF(G10&lt;101,"A",IF(G10="","","ABS"))))))))</f>
+        <v>A</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
+      <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="7">
-        <v>1002340</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7">
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="8">
         <v>5</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="8">
         <v>54</v>
       </c>
       <c r="G11" s="8">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
+      <c r="H11" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
+      <c r="B12" s="2">
         <v>4</v>
       </c>
-      <c r="C12" s="5">
-        <v>1206097</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5">
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="10">
         <v>8</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="10">
         <v>12</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="H12" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+      <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="7">
-        <v>1206096</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7">
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="8">
         <v>6</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="8">
         <v>56</v>
       </c>
       <c r="G13" s="8">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
+      <c r="H13" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="B14" s="2">
         <v>6</v>
       </c>
-      <c r="C14" s="5">
-        <v>1206104</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5">
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="10">
         <v>12</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="10">
         <v>34</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="10">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
+      <c r="H14" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
+      <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="7">
-        <v>1202914</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7">
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="8">
         <v>6</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="8">
         <v>45</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
+      <c r="H15" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
+      <c r="B16" s="2">
         <v>8</v>
       </c>
-      <c r="C16" s="5">
-        <v>1303465</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5">
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="10">
         <v>5</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="10">
         <v>66</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="10">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+      <c r="H16" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
         <v>9</v>
       </c>
-      <c r="C17" s="7">
-        <v>1102303</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7">
+      <c r="C17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8">
         <v>14</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
+      <c r="H17" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
         <v>10</v>
       </c>
-      <c r="C18" s="5">
-        <v>1303439</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5">
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="10">
         <v>0</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="10">
         <v>44</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="10">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
+      <c r="H18" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
         <v>11</v>
       </c>
-      <c r="C19" s="7">
-        <v>1202898</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7">
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="8">
         <v>11</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="8">
         <v>55</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
+      <c r="H19" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
         <v>12</v>
       </c>
-      <c r="C20" s="5">
-        <v>1002339</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5">
+      <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="10">
         <v>2</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="10">
         <v>67</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="10">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
+      <c r="H20" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
         <v>13</v>
       </c>
-      <c r="C21" s="7">
-        <v>1202868</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7">
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="8">
         <v>13</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="8">
         <v>65</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5">
+      <c r="H21" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
         <v>14</v>
       </c>
-      <c r="C22" s="5">
-        <v>1202863</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5">
+      <c r="C22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10">
         <v>34</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="10">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="7">
+      <c r="H22" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
         <v>15</v>
       </c>
-      <c r="C23" s="7">
-        <v>1002361</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7">
+      <c r="C23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8">
         <v>43</v>
       </c>
       <c r="G23" s="8">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
+      <c r="H23" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
         <v>16</v>
       </c>
-      <c r="C24" s="5">
-        <v>1202915</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5">
+      <c r="C24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="10">
         <v>9</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="10">
         <v>23</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="10">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="7">
+      <c r="H24" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
         <v>17</v>
       </c>
-      <c r="C25" s="7">
-        <v>902325</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7">
+      <c r="C25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="8">
         <v>2</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="8">
         <v>53</v>
       </c>
       <c r="G25" s="8">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5">
+      <c r="H25" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
         <v>18</v>
       </c>
-      <c r="C26" s="5">
-        <v>1202878</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5">
+      <c r="C26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="10">
         <v>6</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="10">
         <v>34</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="10">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="7">
+      <c r="H26" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
         <v>19</v>
       </c>
-      <c r="C27" s="7">
-        <v>1202854</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7">
+      <c r="C27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="8">
         <v>8</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="8">
         <v>45</v>
       </c>
       <c r="G27" s="8">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
+      <c r="H27" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
         <v>20</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="2">
         <v>1002345</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5">
+      <c r="D28" s="2"/>
+      <c r="E28" s="10">
         <v>9</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="10">
         <v>65</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="10">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="7">
+      <c r="H28" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
         <v>21</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="3">
         <v>1303420</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7">
+      <c r="D29" s="3"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8">
         <v>15</v>
       </c>
       <c r="G29" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="5">
+      <c r="H29" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
         <v>22</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="2">
         <v>1202882</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5">
+      <c r="D30" s="2"/>
+      <c r="E30" s="10">
         <v>12</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="10">
         <v>53</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="10">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="7">
+      <c r="H30" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
         <v>23</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="3">
         <v>1002302</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7">
+      <c r="D31" s="3"/>
+      <c r="E31" s="8">
         <v>8</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="8">
         <v>34</v>
       </c>
       <c r="G31" s="8">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="5">
+      <c r="H31" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
         <v>24</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="2">
         <v>1206095</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5">
+      <c r="D32" s="2"/>
+      <c r="E32" s="10">
         <v>6</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="10">
         <v>45</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="10">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="7">
+      <c r="H32" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
         <v>25</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="3">
         <v>310348</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7">
+      <c r="D33" s="3"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8">
         <v>65</v>
       </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="5">
+      <c r="H33" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
         <v>26</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="2">
         <v>1202870</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5">
+      <c r="D34" s="2"/>
+      <c r="E34" s="10">
         <v>7</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="10">
         <v>15</v>
       </c>
-      <c r="G34" s="8">
+      <c r="G34" s="10">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="7">
+      <c r="H34" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
         <v>27</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="3">
         <v>1202885</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7">
+      <c r="D35" s="3"/>
+      <c r="E35" s="8">
         <v>11</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="8">
         <v>53</v>
       </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="5">
+      <c r="H35" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
         <v>28</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="2">
         <v>1202879</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5">
+      <c r="D36" s="2"/>
+      <c r="E36" s="10">
         <v>13</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="10">
         <v>34</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="10">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
+      <c r="H36" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
         <v>29</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="3">
         <v>1202899</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7">
+      <c r="D37" s="3"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8">
         <v>45</v>
       </c>
       <c r="G37" s="8">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="5">
+      <c r="H37" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
         <v>30</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="2">
         <v>1002347</v>
       </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5">
+      <c r="D38" s="2"/>
+      <c r="E38" s="10">
         <v>10</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="10">
         <v>65</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="10">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="7">
+      <c r="H38" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
         <v>31</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="3">
         <v>902341</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7">
+      <c r="D39" s="3"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8">
         <v>15</v>
       </c>
       <c r="G39" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="5">
+      <c r="H39" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
         <v>32</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="2">
         <v>1102360</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5">
+      <c r="D40" s="2"/>
+      <c r="E40" s="10">
         <v>5</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="10">
         <v>53</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="10">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="7">
+      <c r="H40" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
         <v>33</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="3">
         <v>1202891</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7">
+      <c r="D41" s="3"/>
+      <c r="E41" s="8">
         <v>7</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="8">
         <v>34</v>
       </c>
       <c r="G41" s="8">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="5">
+      <c r="H41" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
         <v>34</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="2">
         <v>1202056</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5">
+      <c r="D42" s="2"/>
+      <c r="E42" s="10">
         <v>6</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="10">
         <v>45</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="10">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="7">
+      <c r="H42" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
         <v>35</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="3">
         <v>1303453</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7">
+      <c r="D43" s="3"/>
+      <c r="E43" s="8">
         <v>11</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="8">
         <v>65</v>
       </c>
       <c r="G43" s="8">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="5">
+      <c r="H43" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
         <v>36</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="2">
         <v>1303442</v>
       </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5">
+      <c r="D44" s="2"/>
+      <c r="E44" s="10">
         <v>11</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="10">
         <v>15</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="10">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="7">
+      <c r="H44" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
         <v>37</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="3">
         <v>1303414</v>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7">
+      <c r="D45" s="3"/>
+      <c r="E45" s="8">
         <v>8</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="8">
         <v>53</v>
       </c>
       <c r="G45" s="8">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="5">
+      <c r="H45" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
         <v>38</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="2">
         <v>1307377</v>
       </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5">
+      <c r="D46" s="2"/>
+      <c r="E46" s="10">
         <v>3</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="10">
         <v>34</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="10">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="7">
+      <c r="H46" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
         <v>39</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="3">
         <v>1002375</v>
       </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7">
+      <c r="D47" s="3"/>
+      <c r="E47" s="8">
         <v>3</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="8">
         <v>45</v>
       </c>
       <c r="G47" s="8">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="5">
+      <c r="H47" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
         <v>40</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="2">
         <v>1104544</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5">
+      <c r="D48" s="2"/>
+      <c r="E48" s="10">
         <v>6</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="10">
         <v>65</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="10">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="7">
+      <c r="H48" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="3">
         <v>41</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="3">
         <v>1206103</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7">
+      <c r="D49" s="3"/>
+      <c r="E49" s="8">
         <v>5</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="8">
         <v>15</v>
       </c>
       <c r="G49" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="5">
+      <c r="H49" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
         <v>42</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="2">
         <v>1202874</v>
       </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5">
+      <c r="D50" s="2"/>
+      <c r="E50" s="10">
         <v>8</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F50" s="10">
         <v>53</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="10">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="7">
+      <c r="H50" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="3">
         <v>43</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="3">
         <v>1202857</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7">
+      <c r="D51" s="3"/>
+      <c r="E51" s="8">
         <v>13</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F51" s="8">
         <v>34</v>
       </c>
       <c r="G51" s="8">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="5">
+      <c r="H51" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
         <v>44</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="2">
         <v>1104638</v>
       </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5">
+      <c r="D52" s="2"/>
+      <c r="E52" s="10">
         <v>12</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F52" s="10">
         <v>45</v>
       </c>
-      <c r="G52" s="8">
+      <c r="G52" s="10">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="7">
+      <c r="H52" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
         <v>45</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="3">
         <v>1306662</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7">
+      <c r="D53" s="3"/>
+      <c r="E53" s="8">
         <v>4</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F53" s="8">
         <v>65</v>
       </c>
       <c r="G53" s="8">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="5">
+      <c r="H53" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="2">
         <v>46</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="2">
         <v>1102327</v>
       </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5">
+      <c r="D54" s="2"/>
+      <c r="E54" s="10">
         <v>5</v>
       </c>
-      <c r="F54" s="5">
+      <c r="F54" s="10">
         <v>15</v>
       </c>
-      <c r="G54" s="8">
+      <c r="G54" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="7">
+      <c r="H54" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
         <v>47</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="3">
         <v>1202892</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7">
+      <c r="D55" s="3"/>
+      <c r="E55" s="8">
         <v>3</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F55" s="8">
         <v>34</v>
       </c>
       <c r="G55" s="8">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="5">
+      <c r="H55" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="2">
         <v>48</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C56" s="2">
         <v>1202902</v>
       </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5">
+      <c r="D56" s="2"/>
+      <c r="E56" s="10">
         <v>10</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F56" s="10">
         <v>45</v>
       </c>
-      <c r="G56" s="8">
+      <c r="G56" s="10">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="7">
+      <c r="H56" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="3">
         <v>49</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="3">
         <v>1306666</v>
       </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7">
+      <c r="D57" s="3"/>
+      <c r="E57" s="8">
         <v>3</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F57" s="8">
         <v>65</v>
       </c>
       <c r="G57" s="8">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="5">
+      <c r="H57" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="2">
         <v>59</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="2">
         <v>1202861</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5">
+      <c r="D58" s="2"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10">
         <v>15</v>
       </c>
-      <c r="G58" s="8">
+      <c r="G58" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="7">
+      <c r="H58" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="3">
         <v>50</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="3">
         <v>1102337</v>
       </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7">
+      <c r="D59" s="3"/>
+      <c r="E59" s="8">
         <v>7</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F59" s="8">
         <v>53</v>
       </c>
       <c r="G59" s="8">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="5">
+      <c r="H59" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="2">
         <v>51</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C60" s="2">
         <v>1202913</v>
       </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5">
+      <c r="D60" s="2"/>
+      <c r="E60" s="10">
         <v>9</v>
       </c>
-      <c r="F60" s="5">
+      <c r="F60" s="10">
         <v>34</v>
       </c>
-      <c r="G60" s="8">
+      <c r="G60" s="10">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="7">
+      <c r="H60" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="3">
         <v>53</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="3">
         <v>1202881</v>
       </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7">
+      <c r="D61" s="3"/>
+      <c r="E61" s="8">
         <v>10</v>
       </c>
-      <c r="F61" s="7">
+      <c r="F61" s="8">
         <v>45</v>
       </c>
       <c r="G61" s="8">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="5">
+      <c r="H61" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="2">
         <v>54</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C62" s="2">
         <v>1206102</v>
       </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5">
+      <c r="D62" s="2"/>
+      <c r="E62" s="10">
         <v>11</v>
       </c>
-      <c r="F62" s="5">
+      <c r="F62" s="10">
         <v>65</v>
       </c>
-      <c r="G62" s="8">
+      <c r="G62" s="10">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="7">
+      <c r="H62" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="3">
         <v>55</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="3">
         <v>1303417</v>
       </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7">
+      <c r="D63" s="3"/>
+      <c r="E63" s="8">
         <v>3</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F63" s="8">
         <v>15</v>
       </c>
       <c r="G63" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="5">
+      <c r="H63" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="2">
         <v>56</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="2">
         <v>1202920</v>
       </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5">
+      <c r="D64" s="2"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10">
         <v>13</v>
       </c>
-      <c r="G64" s="8">
+      <c r="G64" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="7">
+      <c r="H64" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="3">
         <v>57</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="3">
         <v>1202916</v>
       </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7">
+      <c r="D65" s="3"/>
+      <c r="E65" s="8">
         <v>6</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F65" s="8">
         <v>34</v>
       </c>
       <c r="G65" s="8">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="5">
+      <c r="H65" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="2">
         <v>58</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="2">
         <v>1303421</v>
       </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5">
+      <c r="D66" s="2"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10">
         <v>45</v>
       </c>
-      <c r="G66" s="8">
+      <c r="G66" s="10">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="7">
+      <c r="H66" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="3">
         <v>59</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="3">
         <v>1202901</v>
       </c>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7">
+      <c r="D67" s="3"/>
+      <c r="E67" s="8">
         <v>4</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F67" s="8">
         <v>65</v>
       </c>
       <c r="G67" s="8">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B68" s="5">
+      <c r="H67" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="2">
         <v>60</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68" s="2">
         <v>1202909</v>
       </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5">
+      <c r="D68" s="2"/>
+      <c r="E68" s="10">
         <v>6</v>
       </c>
-      <c r="F68" s="5">
+      <c r="F68" s="10">
         <v>15</v>
       </c>
-      <c r="G68" s="8">
+      <c r="G68" s="10">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="7">
+      <c r="H68" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="3">
         <v>61</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="3">
         <v>1002351</v>
       </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7">
+      <c r="D69" s="3"/>
+      <c r="E69" s="8">
         <v>4</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F69" s="8">
         <v>53</v>
       </c>
       <c r="G69" s="8">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="5">
+      <c r="H69" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="2">
         <v>62</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C70" s="2">
         <v>1002295</v>
       </c>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5">
+      <c r="D70" s="2"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10">
         <v>34</v>
       </c>
-      <c r="G70" s="8">
+      <c r="G70" s="10">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="7">
+      <c r="H70" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="3">
         <v>63</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="3">
         <v>1002318</v>
       </c>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7">
+      <c r="D71" s="3"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8">
         <v>45</v>
       </c>
       <c r="G71" s="8">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="5">
+      <c r="H71" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="2">
         <v>64</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C72" s="2">
         <v>1202888</v>
       </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5">
+      <c r="D72" s="2"/>
+      <c r="E72" s="10">
         <v>12</v>
       </c>
-      <c r="F72" s="5">
+      <c r="F72" s="10">
         <v>65</v>
       </c>
-      <c r="G72" s="8">
+      <c r="G72" s="10">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="7">
+      <c r="H72" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="3">
         <v>65</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="3">
         <v>1202872</v>
       </c>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7">
+      <c r="D73" s="3"/>
+      <c r="E73" s="8">
         <v>14</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F73" s="8">
         <v>15</v>
       </c>
       <c r="G73" s="8">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="5">
+      <c r="H73" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="2">
         <v>66</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="2">
         <v>801750</v>
       </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5">
+      <c r="D74" s="2"/>
+      <c r="E74" s="10">
         <v>3</v>
       </c>
-      <c r="F74" s="5">
+      <c r="F74" s="10">
         <v>53</v>
       </c>
-      <c r="G74" s="8">
-        <f t="shared" ref="G74:G82" si="1">E74+F74</f>
+      <c r="G74" s="10">
+        <f t="shared" ref="G74:G81" si="2">E74+F74</f>
         <v>56</v>
       </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="7">
+      <c r="H74" s="9" t="str">
+        <f t="shared" ref="H74:H108" si="3">IF(G74="","",IF(G74&lt;40,"F",IF(G74&lt;45,"E",IF(G74&lt;50,"D",IF(G74&lt;60,"C",IF(G74&lt;70,"B",IF(G74&lt;101,"A",IF(G74="","","ABS"))))))))</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="3">
         <v>67</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="3">
         <v>1102338</v>
       </c>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7">
+      <c r="D75" s="3"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8">
         <v>34</v>
       </c>
       <c r="G75" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="5">
+      <c r="H75" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
         <v>68</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="2">
         <v>1206101</v>
       </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5">
+      <c r="D76" s="2"/>
+      <c r="E76" s="10">
         <v>6</v>
       </c>
-      <c r="F76" s="5">
+      <c r="F76" s="10">
         <v>45</v>
       </c>
-      <c r="G76" s="8">
-        <f t="shared" si="1"/>
+      <c r="G76" s="10">
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="7">
+      <c r="H76" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="3">
         <v>69</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="3">
         <v>1202869</v>
       </c>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7">
+      <c r="D77" s="3"/>
+      <c r="E77" s="8">
         <v>9</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F77" s="8">
         <v>65</v>
       </c>
       <c r="G77" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="5">
+      <c r="H77" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="2">
         <v>70</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C78" s="2">
         <v>1102339</v>
       </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5">
+      <c r="D78" s="2"/>
+      <c r="E78" s="10">
         <v>2</v>
       </c>
-      <c r="F78" s="5">
+      <c r="F78" s="10">
         <v>15</v>
       </c>
-      <c r="G78" s="8">
-        <f t="shared" si="1"/>
+      <c r="G78" s="10">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="7">
+      <c r="H78" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="3">
         <v>71</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C79" s="3">
         <v>1106019</v>
       </c>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7">
+      <c r="D79" s="3"/>
+      <c r="E79" s="8">
         <v>7</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F79" s="8">
         <v>65</v>
       </c>
       <c r="G79" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="5">
+      <c r="H79" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="2">
         <v>72</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="2">
         <v>1202853</v>
       </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5">
+      <c r="D80" s="2"/>
+      <c r="E80" s="10">
         <v>8</v>
       </c>
-      <c r="F80" s="5">
+      <c r="F80" s="10">
         <v>15</v>
       </c>
-      <c r="G80" s="8">
-        <f t="shared" si="1"/>
+      <c r="G80" s="10">
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="7">
+      <c r="H80" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="3">
         <v>73</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="3">
         <v>1202884</v>
       </c>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7">
+      <c r="D81" s="3"/>
+      <c r="E81" s="8">
         <v>8</v>
       </c>
-      <c r="F81" s="7">
+      <c r="F81" s="8">
         <v>65</v>
       </c>
       <c r="G81" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="9">
-        <v>74</v>
-      </c>
-      <c r="C82" s="9">
-        <v>1202907</v>
-      </c>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9">
-        <v>4</v>
-      </c>
-      <c r="F82" s="9">
-        <v>15</v>
-      </c>
-      <c r="G82" s="8">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85">
-        <f>AVERAGE(G9:G82)</f>
-        <v>48.135135135135137</v>
+      <c r="H81" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+      <c r="G104" s="10"/>
+      <c r="H104" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+      <c r="G107" s="8"/>
+      <c r="H107" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>10</v>
+      </c>
+      <c r="G118">
+        <f>AVERAGE(G9:G97)</f>
+        <v>48.534246575342465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>